<commit_message>
Chaos done Load and save Replenish
</commit_message>
<xml_diff>
--- a/game_template/model/data/floor builder Level 2.xlsx
+++ b/game_template/model/data/floor builder Level 2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7770" windowHeight="540" tabRatio="904" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7770" windowHeight="540" tabRatio="904" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Reverser" sheetId="33" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4694" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4694" uniqueCount="228">
   <si>
     <t>width</t>
   </si>
@@ -1718,6 +1718,9 @@
   <si>
     <t>Walls</t>
   </si>
+  <si>
+    <t>H</t>
+  </si>
 </sst>
 </file>
 
@@ -1958,21 +1961,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="29">
     <dxf>
       <fill>
         <patternFill>
@@ -4892,12 +4881,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="30" priority="2">
+    <cfRule type="expression" dxfId="28" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="29" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6625,12 +6614,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="8" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8358,12 +8347,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="6" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8376,7 +8365,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AB1" sqref="AB1:AB20"/>
     </sheetView>
   </sheetViews>
@@ -10091,12 +10080,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12246,12 +12235,12 @@
     <sortCondition ref="B2:B65"/>
   </sortState>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K65">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13979,12 +13968,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="28" priority="2">
+    <cfRule type="expression" dxfId="26" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="27" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13997,7 +13986,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AB20" sqref="AB1:AB20"/>
     </sheetView>
   </sheetViews>
@@ -15416,7 +15405,7 @@
         <v>11</v>
       </c>
       <c r="S19" s="14" t="s">
-        <v>6</v>
+        <v>227</v>
       </c>
       <c r="T19" s="14" t="s">
         <v>42</v>
@@ -15428,11 +15417,11 @@
       <c r="Y19" s="9"/>
       <c r="AA19" t="str">
         <f t="shared" si="0"/>
-        <v>:\    !!:`:    /:\ !</v>
+        <v>:\    !!:`:    /:\H!</v>
       </c>
       <c r="AB19" t="str">
         <f t="shared" si="1"/>
-        <v>':\    !!:`:    /:\ !',</v>
+        <v>':\    !!:`:    /:\H!',</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
@@ -15713,22 +15702,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y13 A18:Y25 A14:C17 G14:Y17">
-    <cfRule type="expression" dxfId="26" priority="4">
+    <cfRule type="expression" dxfId="24" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z13 A18:Z25 A14:C17 G14:Z17">
-    <cfRule type="cellIs" dxfId="25" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14:F17">
-    <cfRule type="expression" dxfId="24" priority="2">
+    <cfRule type="expression" dxfId="22" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14:F17">
-    <cfRule type="cellIs" dxfId="23" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17456,12 +17445,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="22" priority="2">
+    <cfRule type="expression" dxfId="20" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="21" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19189,12 +19178,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="20" priority="2">
+    <cfRule type="expression" dxfId="18" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="19" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20922,17 +20911,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="18" priority="3">
+    <cfRule type="expression" dxfId="16" priority="3">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="17" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="2" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:M1">
-    <cfRule type="duplicateValues" dxfId="16" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -22658,12 +22647,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="15" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="14" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24391,12 +24380,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="13" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="12" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26124,12 +26113,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>